<commit_message>
- Angular base added - added number of opmerkingen in leerling-dropdown
</commit_message>
<xml_diff>
--- a/docs/import2016.xlsx
+++ b/docs/import2016.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebstormProjects\LLO2016\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebstormProjects\LLO2015\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="0" windowWidth="15195" windowHeight="9495"/>
+    <workbookView xWindow="4875" yWindow="0" windowWidth="15195" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="leerlingen" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="396">
   <si>
     <t>Leerlingnummer</t>
   </si>
@@ -1202,6 +1202,12 @@
   </si>
   <si>
     <t>&lt;option value='CLON'&gt;CLON Grace de Clonie&lt;/option&gt;</t>
+  </si>
+  <si>
+    <t>LLO2016:</t>
+  </si>
+  <si>
+    <t>LLO2015:</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1738,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1758,6 +1764,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2081,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,10 +2150,16 @@
         <f>"{ ""leerling"": { "</f>
         <v xml:space="preserve">{ "leerling": { </v>
       </c>
+      <c r="U1" s="11" t="s">
+        <v>395</v>
+      </c>
       <c r="V1" t="str">
         <f>P1</f>
         <v xml:space="preserve">{ "leerling": { </v>
       </c>
+      <c r="W1" s="11" t="s">
+        <v>394</v>
+      </c>
       <c r="X1" t="str">
         <f>"{ ""leerlingen"": { "</f>
         <v xml:space="preserve">{ "leerlingen": { </v>
@@ -21368,7 +21381,7 @@
         <v>35970</v>
       </c>
       <c r="D194" s="1" t="str">
-        <f t="shared" ref="D194:D257" si="62">+DAY(C194)&amp;"-"&amp;MONTH(C194)&amp;"-"&amp;YEAR(C194)</f>
+        <f t="shared" ref="D194:D249" si="62">+DAY(C194)&amp;"-"&amp;MONTH(C194)&amp;"-"&amp;YEAR(C194)</f>
         <v>24-6-1998</v>
       </c>
       <c r="E194" s="4" t="s">
@@ -21381,7 +21394,7 @@
         <v>26</v>
       </c>
       <c r="H194" t="str">
-        <f t="shared" ref="H194:H257" si="63">+MID(G194,2,2)</f>
+        <f t="shared" ref="H194:H249" si="63">+MID(G194,2,2)</f>
         <v>6V</v>
       </c>
       <c r="I194" t="str">
@@ -21545,7 +21558,7 @@
         <v xml:space="preserve">"leerlingGebdatum": "7-12-1996", </v>
       </c>
       <c r="AE195" t="str">
-        <f t="shared" ref="AE195:AE249" si="78">"""leerlingLeerjaar"": "&amp;+F195&amp;" }, "</f>
+        <f t="shared" ref="AE195:AE248" si="78">"""leerlingLeerjaar"": "&amp;+F195&amp;" }, "</f>
         <v xml:space="preserve">"leerlingLeerjaar": 6 }, </v>
       </c>
       <c r="AF195" t="str">

</xml_diff>